<commit_message>
added taking screenshot after error
</commit_message>
<xml_diff>
--- a/Cena Madery/madera2020.xlsx
+++ b/Cena Madery/madera2020.xlsx
@@ -317,10 +317,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -995,11 +995,11 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2020-01-08</t>
+          <t>2020-01-02</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2345</v>
+        <v>2195</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1010,11 +1010,11 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2020-01-08</t>
+          <t>2020-01-03</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2345</v>
+        <v>2235</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2020-01-08</t>
+          <t>2020-01-07</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1055,11 +1055,11 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2020-01-08</t>
+          <t>2020-01-09</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2345</v>
+        <v>2365</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1070,7 +1070,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2020-01-09</t>
+          <t>2020-01-10</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1085,7 +1085,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2020-01-09</t>
+          <t>2020-01-11</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1100,7 +1100,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2020-01-09</t>
+          <t>2020-01-12</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1109,6 +1109,801 @@
       <c r="C52" t="inlineStr">
         <is>
           <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2020-01-13</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2365</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2020-01-14</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>2365</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2020-01-15</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2315</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2020-01-16</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2020-01-18</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2020-01-19</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2020-01-20</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2020-01-21</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2020-01-22</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2020-01-23</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2415</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2020-01-24</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2515</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2020-01-25</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2515</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2020-01-26</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2515</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2020-01-27</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2515</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2020-01-28</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>2615</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200915050020200915202009222140L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2020-02-04</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2020-02-05</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2020-02-06</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2020-02-07</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2020-02-08</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2020-02-09</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2020-02-10</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2020-02-11</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2020-02-12</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2020-02-13</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2645</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2020-02-14</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>2545</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2020-02-15</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>2545</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2020-02-16</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2545</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2020-02-17</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>2445</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2020-02-18</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>2445</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2020-02-19</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>2445</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2020-02-20</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>2395</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2020-02-21</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>2395</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2020-02-22</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>2395</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2020-02-23</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>2395</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2020-02-24</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2020-02-25</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2020-02-26</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2020-02-27</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2020-02-28</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2020-02-29</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2020-03-01</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2020-03-02</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2020-03-03</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2020-03-04</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2020-03-05</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2020-03-06</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2020-03-07</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>2405</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2020-03-08</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>2405</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2020-03-09</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>2405</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2020-03-10</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>2405</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2020-03-11</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>2405</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.tui.pl/wypoczynek/portugalia/madera/dorisol-florasol-residence-fnc11036/OfferCodeWS/WROFNC20200901044020200901202009082145L07FNC11036STX1GA02</t>
         </is>
       </c>
     </row>

</xml_diff>